<commit_message>
Update dictionaries, correct typos
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/aashtoM145.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/aashtoM145.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997A4CAF-96C7-C242-B7CF-0D4927BAF42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B510CE-A0F8-4046-957A-9502F176F915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -836,9 +836,6 @@
     <t>Well-graded mixture of stone fragments or gravel, coarse sand, fine sand, and a nonplastic or feebly plastic soil binder. This subgroup includes those materials consisting predominantly of coarse sand, either with or without a well-graded soil binder.</t>
   </si>
   <si>
-    <t>Fine beach sand or fine desert blow sand without silty or clay fines or with a very small amount of nonplastic silt. The group includes also streamdeposited mixtures of poorly graded fine sand and limited amounts of coarse sand and gravel.</t>
-  </si>
-  <si>
     <t>A wide variety of “granular” materials that are borderline between the materials falling in Groups A-1 and A-3 and the silt–clay materials of Groups A-4, A-5, A-6, and A-7. This subgroup includes various granular materials containing 35 percent or less passing the 75-μm (No. 200) sieve and with a minus 0.425-mm (No. 40) portion having the characteristics of the A-4  group. These groups include such materialcoarse sand with silt contents or plasticity indexes in excess of the limitations of Group A-1, and fine sand with nonplastic silt content in excess of the limitations of Group A-3.</t>
   </si>
   <si>
@@ -876,6 +873,9 @@
   </si>
   <si>
     <t>DIGGS Soil Classification  Definitions (AASHTO M 145)</t>
+  </si>
+  <si>
+    <t>Fine beach sand or fine desert blow sand without silty or clay fines or with a very small amount of nonplastic silt. The group includes also stream-deposited mixtures of poorly graded fine sand and limited amounts of coarse sand and gravel.</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1634,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1679,10 +1679,10 @@
         <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>235</v>
@@ -1702,8 +1702,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>234</v>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>234</v>
@@ -1810,14 +1810,14 @@
         <v>238</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>234</v>
@@ -1836,14 +1836,14 @@
         <v>239</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>234</v>
@@ -1862,14 +1862,14 @@
         <v>240</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>234</v>
@@ -1888,14 +1888,14 @@
         <v>241</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>234</v>
@@ -1914,14 +1914,14 @@
         <v>242</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>234</v>
@@ -1940,14 +1940,14 @@
         <v>243</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>234</v>
@@ -1966,14 +1966,14 @@
         <v>244</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>234</v>
@@ -1992,14 +1992,14 @@
         <v>245</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>234</v>
@@ -2018,14 +2018,14 @@
         <v>246</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>234</v>
@@ -2044,14 +2044,14 @@
         <v>247</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>234</v>
@@ -2070,14 +2070,14 @@
         <v>248</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>234</v>

</xml_diff>

<commit_message>
Updates to ditionaries and moving pattern files
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/aashtoM145.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/aashtoM145.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B510CE-A0F8-4046-957A-9502F176F915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94638DF-522B-F747-B652-CB0B7B1B93CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19920" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -866,9 +866,6 @@
     <t>Highly organic soils (peat or muck)  based on visual inspection, and are not dependent on percentage passing the 75-μm (No. 200) sieve, liquid limit, or plasticity index. The material is composed primarily of partially decayed organic matter, and generally has a fibrous texture, dark brown or black color, and an odor of decay.</t>
   </si>
   <si>
-    <t>AASHTO D 145</t>
-  </si>
-  <si>
     <t>aashtoM145</t>
   </si>
   <si>
@@ -876,6 +873,9 @@
   </si>
   <si>
     <t>Fine beach sand or fine desert blow sand without silty or clay fines or with a very small amount of nonplastic silt. The group includes also stream-deposited mixtures of poorly graded fine sand and limited amounts of coarse sand and gravel.</t>
+  </si>
+  <si>
+    <t>AASHTO M 145-91</t>
   </si>
 </sst>
 </file>
@@ -1679,10 +1679,10 @@
         <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>235</v>
@@ -1702,8 +1702,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>234</v>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>234</v>
@@ -1810,14 +1810,14 @@
         <v>238</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>234</v>
@@ -1843,7 +1843,7 @@
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>234</v>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>234</v>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>234</v>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>234</v>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>234</v>
@@ -1973,7 +1973,7 @@
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>234</v>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>234</v>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>234</v>
@@ -2051,7 +2051,7 @@
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>234</v>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="14" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>234</v>

</xml_diff>